<commit_message>
Aggiunta di luoghi al primo municipio con zoom modificato
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Capobianco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Capobianco\Desktop\Progetto Ltw\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61470F58-212B-4016-BFD6-C487788A0A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16610902-94CF-44F3-BBE6-9827BE42D965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0B196746-07DA-4CED-8518-28D76236140F}"/>
   </bookViews>
@@ -186,7 +186,6 @@
     <definedName name="ZonaArcheologica">'Municipio I'!$H:$H</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -196,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>.</t>
   </si>
@@ -211,13 +210,103 @@
   </si>
   <si>
     <t>200 gradi</t>
+  </si>
+  <si>
+    <t>Pizza Europa (a viale Europa)</t>
+  </si>
+  <si>
+    <t>GianFornaio</t>
+  </si>
+  <si>
+    <t>Nero lab</t>
+  </si>
+  <si>
+    <t>Baccano</t>
+  </si>
+  <si>
+    <t>Prosciutteria Cantina dei Papi</t>
+  </si>
+  <si>
+    <t>Plant 42</t>
+  </si>
+  <si>
+    <t>Il Veneziano</t>
+  </si>
+  <si>
+    <t>Birra e Spritz</t>
+  </si>
+  <si>
+    <t>Mirto</t>
+  </si>
+  <si>
+    <t>I meet</t>
+  </si>
+  <si>
+    <t>Humus Bistrot</t>
+  </si>
+  <si>
+    <t>Black Market</t>
+  </si>
+  <si>
+    <t>Up sunset bar</t>
+  </si>
+  <si>
+    <t>Salotto 42</t>
+  </si>
+  <si>
+    <t>Cul de Sac</t>
+  </si>
+  <si>
+    <t>Enoteca il Piccolo</t>
+  </si>
+  <si>
+    <t>Taba Café Campo de' Fiori</t>
+  </si>
+  <si>
+    <t>Eretico bistrot</t>
+  </si>
+  <si>
+    <t>Pigna Enoteca di Sardegna</t>
+  </si>
+  <si>
+    <t>Martin Bistrò</t>
+  </si>
+  <si>
+    <t>Bar MART.in.</t>
+  </si>
+  <si>
+    <t>Freeda</t>
+  </si>
+  <si>
+    <t>Dafne Garden Cafè</t>
+  </si>
+  <si>
+    <t>Borgo Ripa</t>
+  </si>
+  <si>
+    <t>L'Oasi della Birra</t>
+  </si>
+  <si>
+    <t>Meccanismo</t>
+  </si>
+  <si>
+    <t>VinAllegro</t>
+  </si>
+  <si>
+    <t>Freni e frizioni</t>
+  </si>
+  <si>
+    <t>Mater Pantheon</t>
+  </si>
+  <si>
+    <t>Polpetta Trastevere</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,9 +315,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -254,10 +357,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -573,29 +677,133 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096AEE50-F225-4C34-A52F-64212300F806}">
   <sheetPr codeName="Foglio1"/>
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="25.77734375" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="I1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I3" t="s">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -701,13 +909,16 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="25.77734375" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
+      <c r="A1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -747,10 +958,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F63257-03FF-4729-B684-5AA863570332}">
   <sheetPr codeName="Foglio5"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="D19" sqref="D1:D1048576"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -760,6 +971,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="19" spans="5:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -813,14 +1049,30 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD63F1E5-72BC-48B9-86F1-7BC00BD6D3E5}">
   <sheetPr codeName="Foglio9"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Municipio III parzialmente finito e ricentrato <3
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Capobianco\Desktop\Progetto Ltw\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47C4285-717C-4F70-9A8E-2C4F3838E856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CBFAFE-AD45-476D-953B-4AFCC01D9A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0B196746-07DA-4CED-8518-28D76236140F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0B196746-07DA-4CED-8518-28D76236140F}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="15" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="176">
   <si>
     <t>Mama Shelter</t>
   </si>
@@ -664,6 +664,87 @@
   </si>
   <si>
     <t>Il Baretto</t>
+  </si>
+  <si>
+    <t>Parsifal Wine Bar Enoteca</t>
+  </si>
+  <si>
+    <t>Apericena</t>
+  </si>
+  <si>
+    <t>BarCiboeEnoteca</t>
+  </si>
+  <si>
+    <t>Roof Cocktail bar</t>
+  </si>
+  <si>
+    <t>Dervock</t>
+  </si>
+  <si>
+    <t>The Random Bar</t>
+  </si>
+  <si>
+    <t>Deriva Aniene - Restaurant, Cocktail bar, Jungle Garden</t>
+  </si>
+  <si>
+    <t>C1b0 Project</t>
+  </si>
+  <si>
+    <t>Drinketto Bistrot</t>
+  </si>
+  <si>
+    <t>Mezzo Litro</t>
+  </si>
+  <si>
+    <t>Enoteca Mostoqui</t>
+  </si>
+  <si>
+    <t>MoVino</t>
+  </si>
+  <si>
+    <t>Beija Flor cocktail bar</t>
+  </si>
+  <si>
+    <t>Bootleg</t>
+  </si>
+  <si>
+    <t>Svago</t>
+  </si>
+  <si>
+    <t>Comò Bistrot</t>
+  </si>
+  <si>
+    <t>Vintro Bar &amp; Bites</t>
+  </si>
+  <si>
+    <t>Danicla Bar</t>
+  </si>
+  <si>
+    <t>Cucci Bistró</t>
+  </si>
+  <si>
+    <t>Talento Bar Gastronomia</t>
+  </si>
+  <si>
+    <t>GALU BAR</t>
+  </si>
+  <si>
+    <t>Mossi Bar</t>
+  </si>
+  <si>
+    <t>Café Les Amì - Caffè e Cucina secondo natura</t>
+  </si>
+  <si>
+    <t>Flora Roma</t>
+  </si>
+  <si>
+    <t>Bar Plaza Caffetteria</t>
+  </si>
+  <si>
+    <t>Bollicina</t>
+  </si>
+  <si>
+    <t>Blink</t>
   </si>
 </sst>
 </file>
@@ -713,11 +794,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1441,8 +1521,8 @@
   <sheetPr codeName="Foglio2"/>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1459,7 +1539,7 @@
       <c r="B1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1739,15 +1819,139 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C260710D-4074-4EAA-9B29-0430C5BE4E2F}">
   <sheetPr codeName="Foglio17"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" activeCellId="1" sqref="B8 B1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="25.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
MILLE COMMIT MA RISOLTOOOOOO
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CE874B-8C9D-497E-AD9E-C8378E513489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34F0B6B-0C60-4E1A-907E-6E85645C95CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="281">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -226,12 +226,6 @@
   </si>
   <si>
     <t>Plant 42</t>
-  </si>
-  <si>
-    <t>Il Veneziano</t>
-  </si>
-  <si>
-    <t>Birra e Spritz</t>
   </si>
   <si>
     <t>Mirto</t>
@@ -881,6 +875,186 @@
   </si>
   <si>
     <t xml:space="preserve">Deriva Aniene </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar Sciubba </t>
+  </si>
+  <si>
+    <t>Fucina Alessandrina</t>
+  </si>
+  <si>
+    <t>Pigneto Cafe' &amp; Spirits</t>
+  </si>
+  <si>
+    <t>L’Ombralonga dal Veneziano</t>
+  </si>
+  <si>
+    <t>Gran Caffè Alessandrino Roma</t>
+  </si>
+  <si>
+    <t>Pigneto Quarantuno</t>
+  </si>
+  <si>
+    <t>BirrEspritz</t>
+  </si>
+  <si>
+    <t>Bar Mosca</t>
+  </si>
+  <si>
+    <t>Pigneto 32</t>
+  </si>
+  <si>
+    <t>New Bar Di Rinaldi Marco</t>
+  </si>
+  <si>
+    <t>The street of crocodiles</t>
+  </si>
+  <si>
+    <t>Bar Sonia</t>
+  </si>
+  <si>
+    <t>Cargo al Pigneto</t>
+  </si>
+  <si>
+    <t>Mad Hop</t>
+  </si>
+  <si>
+    <t>Roxy Bar</t>
+  </si>
+  <si>
+    <t>FricciCore</t>
+  </si>
+  <si>
+    <t>IL Quadrifoglio d'oro</t>
+  </si>
+  <si>
+    <t>Quello - Ristorante Cocktail Bar</t>
+  </si>
+  <si>
+    <t>Cama Centocelle</t>
+  </si>
+  <si>
+    <t>AL PICCOLO VINERIA</t>
+  </si>
+  <si>
+    <t>Da Mario al Pigneto</t>
+  </si>
+  <si>
+    <t>Circolo Artenoize</t>
+  </si>
+  <si>
+    <t>Blue Ice</t>
+  </si>
+  <si>
+    <t>Malavite Roma Pigneto</t>
+  </si>
+  <si>
+    <t>Enoteca Peccati</t>
+  </si>
+  <si>
+    <t>Ape Gourmet</t>
+  </si>
+  <si>
+    <t>Vrasciò</t>
+  </si>
+  <si>
+    <t>Evergreen Centocelle</t>
+  </si>
+  <si>
+    <t>Giolli Bar Roma</t>
+  </si>
+  <si>
+    <t>NABIL</t>
+  </si>
+  <si>
+    <t>Woods Lounge Bar - Centocelle</t>
+  </si>
+  <si>
+    <t>Viveri</t>
+  </si>
+  <si>
+    <t>Glu Glu Roma non solo enoteca</t>
+  </si>
+  <si>
+    <t>Magnebevo e sto al Pigneto</t>
+  </si>
+  <si>
+    <t>Matayaya Ristopub</t>
+  </si>
+  <si>
+    <t>Birra +</t>
+  </si>
+  <si>
+    <t>Retrogusto</t>
+  </si>
+  <si>
+    <t>Bar Rosi Pigneto</t>
+  </si>
+  <si>
+    <t>Sparwasser</t>
+  </si>
+  <si>
+    <t>Pluma</t>
+  </si>
+  <si>
+    <t>Spirito Pigneto</t>
+  </si>
+  <si>
+    <t>Al Turacciolo</t>
+  </si>
+  <si>
+    <t>Hopster</t>
+  </si>
+  <si>
+    <t>Un caffettino?</t>
+  </si>
+  <si>
+    <t>Casa Mangiacotti</t>
+  </si>
+  <si>
+    <t>RED.</t>
+  </si>
+  <si>
+    <t>Zazie nel metrò</t>
+  </si>
+  <si>
+    <t>Caffè Point</t>
+  </si>
+  <si>
+    <t>Garden Bar</t>
+  </si>
+  <si>
+    <t>Il Posto Che Non C'era</t>
+  </si>
+  <si>
+    <t>C'era una volta il caffè villa gordiani</t>
+  </si>
+  <si>
+    <t>Du' Parole</t>
+  </si>
+  <si>
+    <t>La Nave Del Luppolo</t>
+  </si>
+  <si>
+    <t>Cocktail Bar Gelateria L'incontro</t>
+  </si>
+  <si>
+    <t>Long Island</t>
+  </si>
+  <si>
+    <t>Mr.Drink Centocelle</t>
+  </si>
+  <si>
+    <t>Eden Bar Roma</t>
+  </si>
+  <si>
+    <t>Kokus Bar</t>
+  </si>
+  <si>
+    <t>Bar 3M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KRAM </t>
   </si>
 </sst>
 </file>
@@ -942,7 +1116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -951,16 +1125,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1277,87 +1446,87 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
@@ -1365,10 +1534,10 @@
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
@@ -1376,10 +1545,10 @@
     </row>
     <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
@@ -1387,175 +1556,175 @@
     </row>
     <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1688,7 +1857,7 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1699,280 +1868,280 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E22" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1988,7 +2157,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1999,174 +2168,174 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>209</v>
+        <v>34</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2195,183 +2364,183 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>212</v>
+        <v>20</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="7" t="s">
-        <v>213</v>
+      <c r="B14" s="4" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="7"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
-      <c r="B18" s="7"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
-      <c r="B22" s="7"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="7"/>
+      <c r="B27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2384,42 +2553,323 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:B5"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
+      <c r="C5" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
non li avevo messi in verde uff
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56197A7-DBEF-4625-A99E-4431FBC6FD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279EAA02-3FFB-46C1-8390-2D86DD6AD50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="287">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>Officine Beat</t>
-  </si>
-  <si>
-    <t>Gelato Sicily</t>
   </si>
   <si>
     <t>Gli Spritzzati Vino e Cicchetti</t>
@@ -1469,87 +1466,87 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
@@ -1557,10 +1554,10 @@
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>2</v>
@@ -1568,10 +1565,10 @@
     </row>
     <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
@@ -1579,175 +1576,175 @@
     </row>
     <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1891,280 +1888,280 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="17" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="18" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="19" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="22" spans="4:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E22" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2180,7 +2177,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2191,177 +2188,177 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2377,7 +2374,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B1" sqref="B1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2390,153 +2387,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>282</v>
-      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>208</v>
       </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>209</v>
       </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
@@ -2588,7 +2594,6 @@
     </row>
     <row r="27" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2616,300 +2621,300 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>

</xml_diff>

<commit_message>
non so che commit sia
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279EAA02-3FFB-46C1-8390-2D86DD6AD50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A276D2-E62E-427F-B3B2-7EA1CDCFC69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="288">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1073,6 +1073,9 @@
   </si>
   <si>
     <t>Bar Celestino</t>
+  </si>
+  <si>
+    <t>CIACCO - Emporio</t>
   </si>
 </sst>
 </file>
@@ -2374,7 +2377,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2515,6 +2518,9 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>207</v>
       </c>
@@ -2932,7 +2938,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -2947,7 +2955,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
solo excel manco finito ma quanto cazzo è grande il 7 municipio
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A276D2-E62E-427F-B3B2-7EA1CDCFC69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B67DE00-E692-47EF-B29C-9BD885E8796C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="327">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1076,6 +1076,123 @@
   </si>
   <si>
     <t>CIACCO - Emporio</t>
+  </si>
+  <si>
+    <t>Tira e molla</t>
+  </si>
+  <si>
+    <t>Bruni Bistrot Cocktail Bar</t>
+  </si>
+  <si>
+    <t>Salotto Stadlin</t>
+  </si>
+  <si>
+    <t>BAR BRINDISI</t>
+  </si>
+  <si>
+    <t>Le Foodie Café Bistrot</t>
+  </si>
+  <si>
+    <t>Blind Pig</t>
+  </si>
+  <si>
+    <t>VERSO Eatery &amp; Wine Tales</t>
+  </si>
+  <si>
+    <t>C'era una volta il Caffé</t>
+  </si>
+  <si>
+    <t>Piano C - Circolo del vino</t>
+  </si>
+  <si>
+    <t>Sapori e Parole</t>
+  </si>
+  <si>
+    <t>FloW</t>
+  </si>
+  <si>
+    <t>Spigolo</t>
+  </si>
+  <si>
+    <t>Babù</t>
+  </si>
+  <si>
+    <t>malti&amp;mosti</t>
+  </si>
+  <si>
+    <t>Happy Wine Roma</t>
+  </si>
+  <si>
+    <t>Al Solito Posto</t>
+  </si>
+  <si>
+    <t>NaBi Happiness Factory</t>
+  </si>
+  <si>
+    <t>TEO'S - Piazza dell'Alberone</t>
+  </si>
+  <si>
+    <t>Kubla/Khan</t>
+  </si>
+  <si>
+    <t>Quality to Drink</t>
+  </si>
+  <si>
+    <t>Enoteca Bonomi</t>
+  </si>
+  <si>
+    <t>Les Amis</t>
+  </si>
+  <si>
+    <t>QIX drink bar</t>
+  </si>
+  <si>
+    <t>Caffedotto Roma</t>
+  </si>
+  <si>
+    <t>SECONDO GIRO</t>
+  </si>
+  <si>
+    <t>Officina del Sapore</t>
+  </si>
+  <si>
+    <t>Barley Wine</t>
+  </si>
+  <si>
+    <t>Sottosopra</t>
+  </si>
+  <si>
+    <t>Vinum Est Roma</t>
+  </si>
+  <si>
+    <t>La dolce vita</t>
+  </si>
+  <si>
+    <t>Cocktail Bar 23 &amp; Food</t>
+  </si>
+  <si>
+    <t>La Bonora</t>
+  </si>
+  <si>
+    <t>Démodé</t>
+  </si>
+  <si>
+    <t>Rab</t>
+  </si>
+  <si>
+    <t>SpaccioVino Tuscolana</t>
+  </si>
+  <si>
+    <t>Happy Wine </t>
+  </si>
+  <si>
+    <t>Maat Bakery &amp; Bistrot</t>
+  </si>
+  <si>
+    <t>Rquadro</t>
+  </si>
+  <si>
+    <t>Sicilian’s gourmet</t>
   </si>
 </sst>
 </file>
@@ -2376,7 +2493,7 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -2615,7 +2732,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2953,15 +3070,365 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="3" customWidth="1"/>
+    <col min="3" max="6" width="25.21875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ma non avevo fatto commit?
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B67DE00-E692-47EF-B29C-9BD885E8796C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E289F3-B1FC-4B43-A423-D5679E7C316A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <definedName name="AppiaAnticaSud">#REF!</definedName>
     <definedName name="Appio">#REF!</definedName>
     <definedName name="Appio_Claudio">'Municipio VII'!$C:$C</definedName>
-    <definedName name="Appio_Latino7">'Municipio VII'!$F:$F</definedName>
+    <definedName name="Appio_Latino7">'Municipio VII'!$E:$E</definedName>
     <definedName name="Appio_Latino8">'Municipio VIII'!$A:$A</definedName>
     <definedName name="Appio_Pignatelli">'Municipio VIII'!$C:$C</definedName>
     <definedName name="AppioClaudio">#REF!</definedName>
@@ -52,7 +52,7 @@
     <definedName name="Aventino">'Municipio I'!#REF!</definedName>
     <definedName name="Barcaccia">#REF!</definedName>
     <definedName name="Boccea">#REF!</definedName>
-    <definedName name="Borghesiana">'Municipio VII'!$D:$D</definedName>
+    <definedName name="Borghesiana">'Municipio VII'!#REF!</definedName>
     <definedName name="Bufalotta">#REF!</definedName>
     <definedName name="BuonPastore">#REF!</definedName>
     <definedName name="CasalBertone">#REF!</definedName>
@@ -121,7 +121,7 @@
     <definedName name="Morena">#REF!</definedName>
     <definedName name="Navigatori">#REF!</definedName>
     <definedName name="Nomentano">'Municipio II'!$E:$E</definedName>
-    <definedName name="NoName">'Municipio VII'!$E:$E</definedName>
+    <definedName name="NoName">'Municipio VII'!$D:$D</definedName>
     <definedName name="Omo">#REF!</definedName>
     <definedName name="OsteriadelCurato">#REF!</definedName>
     <definedName name="OstiaAntica">#REF!</definedName>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="339">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1193,6 +1193,42 @@
   </si>
   <si>
     <t>Sicilian’s gourmet</t>
+  </si>
+  <si>
+    <t>Fermentum</t>
+  </si>
+  <si>
+    <t>spillo</t>
+  </si>
+  <si>
+    <t>Hopificio</t>
+  </si>
+  <si>
+    <t>Rebacco</t>
+  </si>
+  <si>
+    <t>Ristorante Buono Enoteca e Cocktail Bar</t>
+  </si>
+  <si>
+    <t>Dom</t>
+  </si>
+  <si>
+    <t>Due Punto Zero</t>
+  </si>
+  <si>
+    <t>Perlage</t>
+  </si>
+  <si>
+    <t>Mister TAMO</t>
+  </si>
+  <si>
+    <t>Ma SI! Bar Tavola Calda</t>
+  </si>
+  <si>
+    <t>N°1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buddha Smile </t>
   </si>
 </sst>
 </file>
@@ -3070,21 +3106,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A26" sqref="A1:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.44140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" style="3" customWidth="1"/>
-    <col min="3" max="6" width="25.21875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="3" max="4" width="25.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.5546875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>288</v>
       </c>
@@ -3094,13 +3131,14 @@
       <c r="C1" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>289</v>
       </c>
@@ -3110,13 +3148,14 @@
       <c r="C2" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>290</v>
       </c>
@@ -3126,13 +3165,14 @@
       <c r="C3" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>291</v>
       </c>
@@ -3140,11 +3180,14 @@
       <c r="C4" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>292</v>
       </c>
@@ -3152,11 +3195,14 @@
       <c r="C5" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>293</v>
       </c>
@@ -3164,11 +3210,14 @@
       <c r="C6" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>294</v>
       </c>
@@ -3176,11 +3225,12 @@
       <c r="C7" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>295</v>
       </c>
@@ -3190,19 +3240,19 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>296</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>297</v>
       </c>
@@ -3210,9 +3260,8 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>298</v>
       </c>
@@ -3220,9 +3269,8 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -3230,9 +3278,8 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>300</v>
       </c>
@@ -3240,9 +3287,8 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>301</v>
       </c>
@@ -3250,9 +3296,8 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>302</v>
       </c>
@@ -3260,9 +3305,8 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>304</v>
       </c>
@@ -3270,9 +3314,8 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>305</v>
       </c>
@@ -3280,9 +3323,8 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>306</v>
       </c>
@@ -3290,9 +3332,8 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>307</v>
       </c>
@@ -3300,9 +3341,8 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>309</v>
       </c>
@@ -3310,9 +3350,8 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>311</v>
       </c>
@@ -3320,9 +3359,8 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>312</v>
       </c>
@@ -3330,9 +3368,8 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>313</v>
       </c>
@@ -3340,9 +3377,8 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>314</v>
       </c>
@@ -3350,9 +3386,8 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>315</v>
       </c>
@@ -3360,71 +3395,64 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
quanto è grande il 7 municipio
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E289F3-B1FC-4B43-A423-D5679E7C316A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479ABA6E-DD85-44C3-97F4-40C51E0B9B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="341">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1229,6 +1229,12 @@
   </si>
   <si>
     <t xml:space="preserve">Buddha Smile </t>
+  </si>
+  <si>
+    <t>Room 1.10</t>
+  </si>
+  <si>
+    <t>Baguetteria del Fico</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1306,6 +1312,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1611,9 +1618,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1858,50 +1867,58 @@
         <v>191</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>200</v>
       </c>
+    </row>
+    <row r="42" spans="1:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2330,10 +2347,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2515,6 +2532,11 @@
     <row r="26" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -3108,9 +3130,7 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A1:A26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
vari fix e foto e link
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479ABA6E-DD85-44C3-97F4-40C51E0B9B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDB5CC6-5EF1-4281-9710-8035F958D129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="1" r:id="rId1"/>
@@ -1241,7 +1241,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1267,6 +1267,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1296,7 +1316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1313,6 +1333,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1620,7 +1647,7 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -3130,349 +3157,351 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="3" customWidth="1"/>
-    <col min="3" max="4" width="25.21875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.5546875" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="24.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="9" customWidth="1"/>
+    <col min="3" max="4" width="25.21875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="33.5546875" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="8" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="8" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="8" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
boh non so che commit sia
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12358CF-8AAD-4D7C-92AD-23FB6CA4D4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9467DD7-F0F4-4000-B853-4FCDD876CE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <definedName name="AeroportodellUrbe">#REF!</definedName>
     <definedName name="Alessandrina">#REF!</definedName>
     <definedName name="Alessandrino">'Municipio V'!$C:$C</definedName>
+    <definedName name="Altro">'Municipio X'!$A:$A</definedName>
     <definedName name="AppiaAnticaNord">#REF!</definedName>
     <definedName name="AppiaAnticaSud">#REF!</definedName>
     <definedName name="Appio">#REF!</definedName>
@@ -106,6 +107,7 @@
     <definedName name="LaStorta">#REF!</definedName>
     <definedName name="Latino">#REF!</definedName>
     <definedName name="Laurentino">#REF!</definedName>
+    <definedName name="LidoDIOstia_Ponente">'Municipio X'!$B:$B</definedName>
     <definedName name="LucreziaRomana">#REF!</definedName>
     <definedName name="Lunghezza">#REF!</definedName>
     <definedName name="Magliana">#REF!</definedName>
@@ -196,6 +198,7 @@
     <definedName name="Tuscolano">'Municipio VII'!$A:$A</definedName>
     <definedName name="TuscolanoNord">#REF!</definedName>
     <definedName name="TuscolanoSud">#REF!</definedName>
+    <definedName name="UnicoQuartire">'Municipio X'!$A:$A</definedName>
     <definedName name="Universita">'Municipio II'!$I:$I</definedName>
     <definedName name="ValCannuta">#REF!</definedName>
     <definedName name="ValcoSanPaolo">#REF!</definedName>
@@ -211,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="485">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1571,6 +1574,102 @@
   </si>
   <si>
     <t>Nero.Lab</t>
+  </si>
+  <si>
+    <t>Vineria Anzuini</t>
+  </si>
+  <si>
+    <t>Andreotti - Fonte Meravigliosa</t>
+  </si>
+  <si>
+    <t>Bistrò 65</t>
+  </si>
+  <si>
+    <t>OTTIMO Caffè &amp; Cucina</t>
+  </si>
+  <si>
+    <t>Signorvino</t>
+  </si>
+  <si>
+    <t>Puglià_Maximo</t>
+  </si>
+  <si>
+    <t>Latte e Fondente</t>
+  </si>
+  <si>
+    <t>BLounge Restaurant &amp; Cocktail bar</t>
+  </si>
+  <si>
+    <t>Dolceamaro</t>
+  </si>
+  <si>
+    <t>King's Bistrot</t>
+  </si>
+  <si>
+    <t>Tatti bar</t>
+  </si>
+  <si>
+    <t>Flo_flower_bar</t>
+  </si>
+  <si>
+    <t>Bottega del Buongustaio</t>
+  </si>
+  <si>
+    <t>Mawi</t>
+  </si>
+  <si>
+    <t>IL BAR DEI PARCHI</t>
+  </si>
+  <si>
+    <t>Nero Lab Infernetto</t>
+  </si>
+  <si>
+    <t>ICarusO Casalpalocco</t>
+  </si>
+  <si>
+    <t>Convivium</t>
+  </si>
+  <si>
+    <t>19.2 Winebar Enoteca</t>
+  </si>
+  <si>
+    <t>Enoteca Versatile</t>
+  </si>
+  <si>
+    <t>Shilling</t>
+  </si>
+  <si>
+    <t>Open Bar</t>
+  </si>
+  <si>
+    <t>MAGA Wine Bar - Cucina di Mare</t>
+  </si>
+  <si>
+    <t>Sandrino's</t>
+  </si>
+  <si>
+    <t>Mas Magna e Bevi</t>
+  </si>
+  <si>
+    <t>Bahia beach Bar</t>
+  </si>
+  <si>
+    <t>ALWINE</t>
+  </si>
+  <si>
+    <t>Insolito Food &amp; Drink Lido di Ostia</t>
+  </si>
+  <si>
+    <t>Il Sole di Ostia</t>
+  </si>
+  <si>
+    <t>Pachamama Beachbar</t>
+  </si>
+  <si>
+    <t>La Spiaggia </t>
+  </si>
+  <si>
+    <t>V Lounge Beach</t>
   </si>
 </sst>
 </file>
@@ -2313,12 +2412,242 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="30.88671875" style="12" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4477,8 +4806,8 @@
   </sheetPr>
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4489,172 +4818,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="8" t="s">
+        <v>458</v>
+      </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="8" t="s">
+        <v>459</v>
+      </c>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="11"/>
     </row>
     <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="11"/>
     </row>
     <row r="19" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="11"/>
     </row>
     <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="B20" s="11"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="11"/>
     </row>
     <row r="21" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="11"/>
     </row>
     <row r="22" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="B22" s="11"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B23" s="8"/>
       <c r="C23" s="11"/>
     </row>
     <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="B24" s="8"/>
       <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="B25" s="8"/>
       <c r="C25" s="11"/>
     </row>
     <row r="26" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
dodici ma mancano le coordinate, devo andare a fare ripe le aggiungo stasera
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D9E6F0-9095-44CF-96FC-A0F61359A4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0642C281-6369-41E4-B368-A685A05A5C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="514">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1700,6 +1700,63 @@
   </si>
   <si>
     <t>Bar India</t>
+  </si>
+  <si>
+    <t>Enoteca - I Figli del Vinaio</t>
+  </si>
+  <si>
+    <t>KilometroZERO Coffee, Drink&amp;Food</t>
+  </si>
+  <si>
+    <t>Totem Garden Bar</t>
+  </si>
+  <si>
+    <t>Santa Maria Bar &amp; Bistrot</t>
+  </si>
+  <si>
+    <t>Cafe Vert</t>
+  </si>
+  <si>
+    <t>Matière | Bar-à-vin</t>
+  </si>
+  <si>
+    <t>Massimi Caffè</t>
+  </si>
+  <si>
+    <t>Caffè 104</t>
+  </si>
+  <si>
+    <t>Bar Faustini</t>
+  </si>
+  <si>
+    <t>Off Living Room</t>
+  </si>
+  <si>
+    <t>Giano Bistrot</t>
+  </si>
+  <si>
+    <t>Think Farmer</t>
+  </si>
+  <si>
+    <t>HÉCO Trastevere</t>
+  </si>
+  <si>
+    <t>Gianicolo Garden</t>
+  </si>
+  <si>
+    <t>Friccico Mangia&amp;Bevi Bistrò</t>
+  </si>
+  <si>
+    <t>BistrOUT</t>
+  </si>
+  <si>
+    <t>Il Pozzo since 1973 Roma</t>
+  </si>
+  <si>
+    <t>Cortile Bravetta</t>
+  </si>
+  <si>
+    <t>Bistrot Enoteca ai Colli</t>
   </si>
 </sst>
 </file>
@@ -2445,7 +2502,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2689,8 +2746,8 @@
   </sheetPr>
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2909,12 +2966,223 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.5546875" style="12" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>501</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>502</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>511</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5044,7 +5312,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Mama Shelter sta a trionfale non a prati
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCF9434-39BF-43CB-A5FC-22C6D5357D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7523CAC-B4BE-4ACD-8F8C-DB3FF04809BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Municipio I" sheetId="1" r:id="rId1"/>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="539">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1820,6 +1820,18 @@
   </si>
   <si>
     <t>Enoteca dei Desideri</t>
+  </si>
+  <si>
+    <t>VIVI - Le serre</t>
+  </si>
+  <si>
+    <t>VINNICO Wine Bar</t>
+  </si>
+  <si>
+    <t>CHYMEIA - Cocktail Bar &amp; Gastro Miscelazione</t>
+  </si>
+  <si>
+    <t>Café Gourmet</t>
   </si>
 </sst>
 </file>
@@ -2253,7 +2265,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2268,9 +2280,6 @@
       </c>
       <c r="B1" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -3258,8 +3267,8 @@
   </sheetPr>
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3500,12 +3509,206 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.5546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" style="12" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
mi si sta scaricando il computer, domani faccio il 15
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7523CAC-B4BE-4ACD-8F8C-DB3FF04809BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0961402-DD01-4AF7-9CCC-15F41E377D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="555">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1832,6 +1832,54 @@
   </si>
   <si>
     <t>Café Gourmet</t>
+  </si>
+  <si>
+    <t>Craft House</t>
+  </si>
+  <si>
+    <t>Pane e Salame F.lli Lattanzi – Torrevecchia</t>
+  </si>
+  <si>
+    <t>Piso 35 PUB &amp; Beer Bakery</t>
+  </si>
+  <si>
+    <t>Hic - Vizi &amp; Sfizi</t>
+  </si>
+  <si>
+    <t>Caffè Letterario e Aperitivi Roma | Macondo</t>
+  </si>
+  <si>
+    <t>Bar Sicilia</t>
+  </si>
+  <si>
+    <t>Bar Pasticceria Dolce Oasi</t>
+  </si>
+  <si>
+    <t>Festival Snack Bar</t>
+  </si>
+  <si>
+    <t>Mezzanottetre</t>
+  </si>
+  <si>
+    <t>Enoteca DivinEmozioni</t>
+  </si>
+  <si>
+    <t>Bar Cheri 2</t>
+  </si>
+  <si>
+    <t>Four Sisters</t>
+  </si>
+  <si>
+    <t>Black'n White</t>
+  </si>
+  <si>
+    <t>Foodoo</t>
+  </si>
+  <si>
+    <t>Cafe Porteño</t>
+  </si>
+  <si>
+    <t>Caffè La Terrazza</t>
   </si>
 </sst>
 </file>
@@ -3512,86 +3560,120 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A13" sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="38" style="12" customWidth="1"/>
     <col min="2" max="2" width="39.5546875" style="12" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
+      <c r="A1" s="11" t="s">
+        <v>539</v>
+      </c>
       <c r="B1" s="11" t="s">
         <v>140</v>
       </c>
       <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
+      <c r="A2" s="11" t="s">
+        <v>540</v>
+      </c>
       <c r="B2" s="11" t="s">
         <v>535</v>
       </c>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
+      <c r="A3" s="11" t="s">
+        <v>541</v>
+      </c>
       <c r="B3" s="11" t="s">
         <v>536</v>
       </c>
       <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="11" t="s">
+        <v>542</v>
+      </c>
       <c r="B4" s="11" t="s">
         <v>537</v>
       </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="11" t="s">
+        <v>543</v>
+      </c>
       <c r="B5" s="11" t="s">
         <v>538</v>
       </c>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>552</v>
+      </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="11"/>
+      <c r="A7" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>553</v>
+      </c>
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
+      <c r="A8" s="11" t="s">
+        <v>546</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>554</v>
+      </c>
       <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
+      <c r="A9" s="11" t="s">
+        <v>547</v>
+      </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="A10" s="11" t="s">
+        <v>548</v>
+      </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
+      <c r="A11" s="11" t="s">
+        <v>549</v>
+      </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+      <c r="A12" s="11" t="s">
+        <v>550</v>
+      </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
+      <c r="A13" s="11" t="s">
+        <v>551</v>
+      </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
     </row>
@@ -3710,6 +3792,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5799,7 +5882,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
QUATTORDICI a sto giro mi so ricordata di centrare
</commit_message>
<xml_diff>
--- a/ElencoLuoghi.xlsx
+++ b/ElencoLuoghi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB-CASA\OneDrive - SOGETEL srl\Desktop\UNI_Laura\ProgettoLTW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0961402-DD01-4AF7-9CCC-15F41E377D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B74547-C714-49BE-88DD-BBBE2F63E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="559">
   <si>
     <t>Quintessenza</t>
   </si>
@@ -1880,6 +1880,18 @@
   </si>
   <si>
     <t>Caffè La Terrazza</t>
+  </si>
+  <si>
+    <t>Fábrica</t>
+  </si>
+  <si>
+    <t>il Covino</t>
+  </si>
+  <si>
+    <t>The Loft</t>
+  </si>
+  <si>
+    <t>Green Bar</t>
   </si>
 </sst>
 </file>
@@ -3560,7 +3572,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:A13"/>
+      <selection activeCell="B13" sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3571,110 +3583,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>140</v>
       </c>
       <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>535</v>
       </c>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>541</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>536</v>
       </c>
       <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>537</v>
       </c>
       <c r="C4" s="11"/>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>543</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>538</v>
       </c>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>552</v>
       </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>553</v>
       </c>
       <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>546</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>554</v>
       </c>
       <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="8" t="s">
+        <v>555</v>
+      </c>
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="8" t="s">
+        <v>556</v>
+      </c>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="8" t="s">
+        <v>557</v>
+      </c>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="8" t="s">
         <v>550</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="8" t="s">
+        <v>558</v>
+      </c>
       <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>